<commit_message>
implmented visualization and support structure
Visualization serves as the main creater of the Sankey graphic
</commit_message>
<xml_diff>
--- a/CSCohortTest.xlsx
+++ b/CSCohortTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="15">
   <si>
     <t>CS</t>
   </si>
@@ -420,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770929AA-B505-4CBD-982A-8C7E2428B683}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>2017</v>
       </c>
@@ -436,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -453,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -469,8 +469,26 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -486,8 +504,26 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -503,8 +539,26 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -520,8 +574,26 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -537,8 +609,26 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -554,8 +644,26 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -571,8 +679,26 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -588,8 +714,26 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -605,8 +749,26 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -620,6 +782,24 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
concept of permanency of click added
When a major or student is clicked, and the subset grows or shrinks,
that major or student remains clicked
</commit_message>
<xml_diff>
--- a/CSCohortTest.xlsx
+++ b/CSCohortTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="16">
   <si>
     <t>CS</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>FEMALE</t>
+  </si>
+  <si>
+    <t>E64000</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770929AA-B505-4CBD-982A-8C7E2428B683}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K239" sqref="K239"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,22 +613,22 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1431,6 +1434,601 @@
       </c>
       <c r="K30" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" t="s">
+        <v>12</v>
+      </c>
+      <c r="K43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>10</v>
+      </c>
+      <c r="K46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" t="s">
+        <v>10</v>
+      </c>
+      <c r="K47" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leave or remain parameters added, text added to diagram
</commit_message>
<xml_diff>
--- a/CSCohortTest.xlsx
+++ b/CSCohortTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="16">
   <si>
     <t>CS</t>
   </si>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770929AA-B505-4CBD-982A-8C7E2428B683}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2015,20 +2015,20 @@
       <c r="F47" t="s">
         <v>10</v>
       </c>
-      <c r="G47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" t="s">
-        <v>10</v>
-      </c>
-      <c r="I47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J47" t="s">
-        <v>10</v>
-      </c>
-      <c r="K47" t="s">
-        <v>10</v>
+      <c r="G47">
+        <v>605030</v>
+      </c>
+      <c r="H47">
+        <v>605030</v>
+      </c>
+      <c r="I47">
+        <v>605030</v>
+      </c>
+      <c r="J47">
+        <v>605030</v>
+      </c>
+      <c r="K47">
+        <v>605030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>